<commit_message>
The program works now at a basic level
</commit_message>
<xml_diff>
--- a/New Shoes.xlsx
+++ b/New Shoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reed/PycharmProjects/760_Marketing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BD9F89-E97C-6C47-8606-DE74F02249DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64B8E15-3F79-BD46-85E8-3339808E31EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12740" yWindow="13780" windowWidth="21900" windowHeight="8940" xr2:uid="{35ED14CE-7522-5B4E-8ED6-92489854B887}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="3" xr2:uid="{35ED14CE-7522-5B4E-8ED6-92489854B887}"/>
   </bookViews>
   <sheets>
     <sheet name="-1" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="18">
   <si>
     <t>Akili Max</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Corporate</t>
+  </si>
+  <si>
+    <t>Product Level</t>
   </si>
 </sst>
 </file>
@@ -443,76 +446,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666F882C-7748-A54D-AC11-7FB920C28AD3}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -520,22 +529,25 @@
         <v>800000</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>90</v>
       </c>
-      <c r="D3">
-        <v>1000000</v>
-      </c>
       <c r="E3">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F3">
+        <v>2000000</v>
+      </c>
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -543,22 +555,25 @@
         <v>800000</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>90</v>
       </c>
-      <c r="D4">
-        <v>1000000</v>
-      </c>
       <c r="E4">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F4">
+        <v>2000000</v>
+      </c>
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -566,22 +581,25 @@
         <v>800000</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>90</v>
       </c>
-      <c r="D5">
-        <v>1000000</v>
-      </c>
       <c r="E5">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F5">
+        <v>2000000</v>
+      </c>
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="G5">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -589,22 +607,25 @@
         <v>800000</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>90</v>
       </c>
-      <c r="D6">
-        <v>1000000</v>
-      </c>
       <c r="E6">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F6">
+        <v>2000000</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -612,22 +633,25 @@
         <v>800000</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>90</v>
       </c>
-      <c r="D7">
-        <v>1000000</v>
-      </c>
       <c r="E7">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F7">
+        <v>2000000</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="G7">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -635,22 +659,25 @@
         <v>800000</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>90</v>
       </c>
-      <c r="D8">
-        <v>1000000</v>
-      </c>
       <c r="E8">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F8">
+        <v>2000000</v>
+      </c>
+      <c r="G8">
         <v>5</v>
       </c>
-      <c r="G8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -658,25 +685,29 @@
         <v>800000</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>90</v>
       </c>
-      <c r="D9">
-        <v>1000000</v>
-      </c>
       <c r="E9">
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="F9">
+        <v>2000000</v>
+      </c>
+      <c r="G9">
         <v>5</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1000000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:O1"/>
+  <mergeCells count="3">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -684,67 +715,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C03D8580-9FB5-864D-B682-9D20584055D4}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -752,37 +787,40 @@
         <v>900000</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>110</v>
       </c>
-      <c r="D3">
-        <v>1500000</v>
-      </c>
       <c r="E3">
+        <v>1500000</v>
+      </c>
+      <c r="F3">
         <v>2500000</v>
       </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
       <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
         <v>1200000</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>90</v>
       </c>
-      <c r="J3">
-        <v>2000000</v>
-      </c>
       <c r="K3">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L3">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -790,37 +828,40 @@
         <v>900000</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>110</v>
       </c>
-      <c r="D4">
-        <v>1500000</v>
-      </c>
       <c r="E4">
+        <v>1500000</v>
+      </c>
+      <c r="F4">
         <v>2500000</v>
       </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
       <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
         <v>1200000</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>90</v>
       </c>
-      <c r="J4">
-        <v>2000000</v>
-      </c>
       <c r="K4">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L4">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M4">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="N4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -828,37 +869,40 @@
         <v>900000</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>110</v>
       </c>
-      <c r="D5">
-        <v>1500000</v>
-      </c>
       <c r="E5">
+        <v>1500000</v>
+      </c>
+      <c r="F5">
         <v>2500000</v>
       </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
       <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
         <v>1200000</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>90</v>
       </c>
-      <c r="J5">
-        <v>2000000</v>
-      </c>
       <c r="K5">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L5">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M5">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -866,37 +910,40 @@
         <v>900000</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>110</v>
       </c>
-      <c r="D6">
-        <v>1500000</v>
-      </c>
       <c r="E6">
+        <v>1500000</v>
+      </c>
+      <c r="F6">
         <v>2500000</v>
       </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
       <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
         <v>1200000</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>90</v>
       </c>
-      <c r="J6">
-        <v>2000000</v>
-      </c>
       <c r="K6">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L6">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M6">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -904,37 +951,40 @@
         <v>900000</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>110</v>
       </c>
-      <c r="D7">
-        <v>1500000</v>
-      </c>
       <c r="E7">
+        <v>1500000</v>
+      </c>
+      <c r="F7">
         <v>2500000</v>
       </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
       <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
         <v>1200000</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>90</v>
       </c>
-      <c r="J7">
-        <v>2000000</v>
-      </c>
       <c r="K7">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L7">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M7">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -942,37 +992,40 @@
         <v>900000</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>110</v>
       </c>
-      <c r="D8">
-        <v>1500000</v>
-      </c>
       <c r="E8">
+        <v>1500000</v>
+      </c>
+      <c r="F8">
         <v>2500000</v>
       </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
       <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
         <v>1200000</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>90</v>
       </c>
-      <c r="J8">
-        <v>2000000</v>
-      </c>
       <c r="K8">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L8">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -980,104 +1033,114 @@
         <v>900000</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>110</v>
       </c>
-      <c r="D9">
-        <v>1500000</v>
-      </c>
       <c r="E9">
+        <v>1500000</v>
+      </c>
+      <c r="F9">
         <v>2500000</v>
       </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
       <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
         <v>1200000</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>90</v>
       </c>
-      <c r="J9">
-        <v>2000000</v>
-      </c>
       <c r="K9">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L9">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
         <v>1000000</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE93CBA-5A59-464F-AFBB-4769B2CEA28B}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1085,43 +1148,46 @@
         <v>1500000</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>55</v>
       </c>
-      <c r="D3">
-        <v>1000000</v>
-      </c>
       <c r="E3">
+        <v>1000000</v>
+      </c>
+      <c r="F3">
         <v>500000</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>900000</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>77</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>55</v>
       </c>
-      <c r="J3">
-        <v>1000000</v>
-      </c>
       <c r="K3">
+        <v>1000000</v>
+      </c>
+      <c r="L3">
         <v>500000</v>
       </c>
-      <c r="L3">
-        <v>7</v>
-      </c>
       <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
         <v>800000</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1129,43 +1195,46 @@
         <v>950000</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>105</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1200000</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2250000</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="G4">
-        <v>1000000</v>
-      </c>
       <c r="H4">
+        <v>1000000</v>
+      </c>
+      <c r="I4">
         <v>52.8</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>95</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1800000</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1300000</v>
       </c>
-      <c r="L4">
-        <v>7</v>
-      </c>
       <c r="M4">
+        <v>7</v>
+      </c>
+      <c r="N4">
         <v>900000</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>43.4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1173,43 +1242,46 @@
         <v>900000</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>110</v>
       </c>
-      <c r="D5">
-        <v>1500000</v>
-      </c>
       <c r="E5">
+        <v>1500000</v>
+      </c>
+      <c r="F5">
         <v>2500000</v>
       </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
       <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
         <v>1200000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>46.2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>90</v>
       </c>
-      <c r="J5">
-        <v>2000000</v>
-      </c>
       <c r="K5">
-        <v>1500000</v>
+        <v>2000000</v>
       </c>
       <c r="L5">
-        <v>7</v>
+        <v>1500000</v>
       </c>
       <c r="M5">
-        <v>1000000</v>
+        <v>7</v>
       </c>
       <c r="N5">
+        <v>1000000</v>
+      </c>
+      <c r="O5">
         <v>49.1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1217,43 +1289,46 @@
         <v>2000000</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>77.989999999999995</v>
       </c>
-      <c r="D6">
-        <v>2000000</v>
-      </c>
       <c r="E6">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="F6">
+        <v>1000000</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>500000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>77</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>74.989999999999995</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1700000</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>700000</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>10</v>
       </c>
-      <c r="M6">
-        <v>1000000</v>
-      </c>
       <c r="N6">
+        <v>1000000</v>
+      </c>
+      <c r="O6">
         <v>66.7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1261,43 +1336,46 @@
         <v>1350000</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>99.99</v>
       </c>
-      <c r="D7">
-        <v>1500000</v>
-      </c>
       <c r="E7">
-        <v>2000000</v>
+        <v>1500000</v>
       </c>
       <c r="F7">
-        <v>7</v>
+        <v>2000000</v>
       </c>
       <c r="G7">
-        <v>1000000</v>
+        <v>7</v>
       </c>
       <c r="H7">
+        <v>1000000</v>
+      </c>
+      <c r="I7">
         <v>59.4</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>90.99</v>
       </c>
-      <c r="J7">
-        <v>2000000</v>
-      </c>
       <c r="K7">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="L7">
+        <v>1000000</v>
+      </c>
+      <c r="M7">
         <v>9</v>
       </c>
-      <c r="M7">
-        <v>1000000</v>
-      </c>
       <c r="N7">
+        <v>1000000</v>
+      </c>
+      <c r="O7">
         <v>47.9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1305,43 +1383,46 @@
         <v>2000000</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>99.99</v>
       </c>
-      <c r="D8">
-        <v>1000000</v>
-      </c>
       <c r="E8">
-        <v>1500000</v>
+        <v>1000000</v>
       </c>
       <c r="F8">
+        <v>1500000</v>
+      </c>
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="G8">
-        <v>1000000</v>
-      </c>
       <c r="H8">
+        <v>1000000</v>
+      </c>
+      <c r="I8">
         <v>59.4</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>79.989999999999995</v>
       </c>
-      <c r="J8">
-        <v>1000000</v>
-      </c>
       <c r="K8">
         <v>1000000</v>
       </c>
       <c r="L8">
+        <v>1000000</v>
+      </c>
+      <c r="M8">
         <v>8</v>
       </c>
-      <c r="M8">
-        <v>1000000</v>
-      </c>
       <c r="N8">
+        <v>1000000</v>
+      </c>
+      <c r="O8">
         <v>60.8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1349,159 +1430,170 @@
         <v>2000000</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>85</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>850000</v>
       </c>
-      <c r="E9">
-        <v>1000000</v>
-      </c>
       <c r="F9">
+        <v>1000000</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>350000</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>77</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>79</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1250000</v>
       </c>
-      <c r="K9">
-        <v>1000000</v>
-      </c>
       <c r="L9">
+        <v>1000000</v>
+      </c>
+      <c r="M9">
         <v>10</v>
       </c>
-      <c r="M9">
-        <v>1000000</v>
-      </c>
       <c r="N9">
+        <v>1000000</v>
+      </c>
+      <c r="O9">
         <v>62</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825A73BD-E9D2-8148-821A-AACF8208B0E8}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:O1"/>
+  <mergeCells count="3">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>